<commit_message>
added framework for kistrong in Multiplayer and fixed button bug in ki
</commit_message>
<xml_diff>
--- a/Nicht Programm/Fehler.xlsx
+++ b/Nicht Programm/Fehler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Veronika\Documents\GitHub\Schiffe_Versenken\Nicht Programm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\IdeaProjects\Schiffe_Versenken\Nicht Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E358FF98-6E32-4B68-B1EC-A43A242FCA00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC93168F-AC92-41E0-96E8-64FDB6C8A0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{C08E704F-E386-4341-9DA7-5A9736508E88}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C08E704F-E386-4341-9DA7-5A9736508E88}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Priorität</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Optionen im Startscreen sind nicht nutzbar</t>
   </si>
   <si>
-    <t>Auto Btn im KI Multiplayer Spiel tut noch nicht</t>
-  </si>
-  <si>
     <t>Controller_Startscreens</t>
   </si>
   <si>
@@ -172,6 +169,18 @@
   </si>
   <si>
     <t>titel setzen bei Host und Client scene/stage und centrieren wenn in Putship wechselt</t>
+  </si>
+  <si>
+    <t>Falsches ChoiceBox Event in KivsKi, Geschwindigkeit updated beim Klicken auf die Box und nicht auf das Menü</t>
+  </si>
+  <si>
+    <t>Controller_GameScreen</t>
+  </si>
+  <si>
+    <t>Auto Btn im KI Multiplayer Spiel führt zu Fehlern in der Kommunikation tut noch nicht</t>
+  </si>
+  <si>
+    <t>PutShips hängt sich im Multiplayer auf wenn man vor dem Host auf Start drückt</t>
   </si>
 </sst>
 </file>
@@ -576,21 +585,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C048712A-23BE-4482-B80C-405D201BA276}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" customWidth="1"/>
-    <col min="3" max="3" width="36.83984375" customWidth="1"/>
-    <col min="4" max="4" width="31.68359375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.81640625" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -601,10 +610,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -612,176 +621,195 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>4</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
-        <v>9</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="38.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
+    </row>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed to fit new version
</commit_message>
<xml_diff>
--- a/Nicht Programm/Fehler.xlsx
+++ b/Nicht Programm/Fehler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Ulrich\IdeaProjects\Schiffe_Versenken\Nicht Programm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E652AFB8-8209-406C-BD30-9436074C8F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456BBE3B-A9F6-43E2-91A2-F4367305910F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{C08E704F-E386-4341-9DA7-5A9736508E88}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08E704F-E386-4341-9DA7-5A9736508E88}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Priorität</t>
   </si>
@@ -93,33 +93,12 @@
     <t>Methode startGame in GameScreen müsste vermutlichin Controller_PutShips aufgerufen und richtig gethreaded werden</t>
   </si>
   <si>
-    <t>Fenster sollten alle eine gleiche Mindestgröße haben</t>
-  </si>
-  <si>
-    <t>Beim mehrmaligen klicken auf ein zerstörtes Feld im Multiplayer, gewinnt man</t>
-  </si>
-  <si>
-    <t>if statement mit abfrage ob auf ein Feld schonmal geschossen wurde in checkGameEnded (GameScreen) einfügen</t>
-  </si>
-  <si>
-    <t>KI HELL aus den Choiceboxen im Multiplayer rausnehmen</t>
-  </si>
-  <si>
-    <t>Layout_Hostgame &amp; Layout_ClientGame</t>
-  </si>
-  <si>
     <t>Ki Strong führt zu Fehlern im Multiplayer</t>
   </si>
   <si>
     <t>Ki</t>
   </si>
   <si>
-    <t>HostGame kann sich mit einem ClientGame im selben Fenster verbinden, wenn durch back verlassen und anderes aufgerufen wird</t>
-  </si>
-  <si>
-    <t>Back Buttons in Controller_Loading Screen beenden Socket nicht</t>
-  </si>
-  <si>
     <t xml:space="preserve">Schwierigkeit    (eigene Einschätzung) </t>
   </si>
   <si>
@@ -138,51 +117,18 @@
     <t>Programm ausführbar machen (z.b. .exe)</t>
   </si>
   <si>
-    <t xml:space="preserve"> removeAllShips in Field wird nicht benutzt??</t>
-  </si>
-  <si>
     <t>Intelij</t>
   </si>
   <si>
-    <t>Immer beim Scenenwechsel zur GameScreen</t>
-  </si>
-  <si>
-    <t>Nach dem Removen von mehreren Schiffen kann immer nur das zuletzt entfernte Schiff wiedergesetzt werden</t>
-  </si>
-  <si>
-    <t>Controller_Putships: Es würde reichen das längste Schiff immer als erstes in der Liste zu haben, sprich einen if(entferntes Schiff.länge&gt;liste[0].schifflänge-&gt;liste[0]=entferntesSchiff &amp; anderes schiff inserten</t>
-  </si>
-  <si>
-    <t>Muss möglicherweise gelöscht werden</t>
-  </si>
-  <si>
     <t>einfach</t>
   </si>
   <si>
-    <t>titel setzen bei Host und Client scene/stage und centrieren wenn in Putship wechselt</t>
-  </si>
-  <si>
-    <t>Falsches ChoiceBox Event in KivsKi, Geschwindigkeit updated beim Klicken auf die Box und nicht auf das Menü</t>
-  </si>
-  <si>
-    <t>Controller_GameScreen</t>
-  </si>
-  <si>
-    <t>Auto Btn im KI Multiplayer Spiel führt zu Fehlern in der Kommunikation tut noch nicht</t>
-  </si>
-  <si>
     <t>PutShips hängt sich im Multiplayer auf wenn man vor dem Host auf Start drückt</t>
   </si>
   <si>
-    <t>Controller_Gamescreen, könnte Threadingfehler sein; Vermutung Fehler tritt auf wenn während einem laufenden Zug von auto auf manuell gewechselt wird</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mittel </t>
   </si>
   <si>
-    <t xml:space="preserve">Einfach </t>
-  </si>
-  <si>
     <t>HTML Doc Platz klären und vervollständigen</t>
   </si>
   <si>
@@ -195,16 +141,10 @@
     <t>mittel</t>
   </si>
   <si>
-    <t>Speicherfunktionen fertigstellen</t>
-  </si>
-  <si>
-    <t>Startbutton wieder disablen nach remove</t>
-  </si>
-  <si>
-    <t>shootRandom in Range random suchen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beim ersten Schuss im Client Game </t>
+    <t>KivsKi gibt keine Siegesmeldung aus</t>
+  </si>
+  <si>
+    <t>Bei Hell Ki nach jedem Zerstörten Schiff Meldung das sie dir eine Chance lässt</t>
   </si>
 </sst>
 </file>
@@ -241,7 +181,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,13 +190,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,14 +235,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,22 +552,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C048712A-23BE-4482-B80C-405D201BA276}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64" customWidth="1"/>
+    <col min="1" max="1" width="64" style="2" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -649,11 +577,11 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4">
@@ -663,239 +591,98 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="8">
-        <v>2</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
+      <c r="C8" t="s">
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="12">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="4">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="8">
-        <v>2</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>